<commit_message>
Still struggling with data aggregation.
</commit_message>
<xml_diff>
--- a/raw-data-prep/raw_data/Note_sheet_RP.xlsx
+++ b/raw-data-prep/raw_data/Note_sheet_RP.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -39,24 +39,12 @@
     <t>Good Session</t>
   </si>
   <si>
-    <t xml:space="preserve">Notes </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Game 1 </t>
-  </si>
-  <si>
     <t>Game 2</t>
   </si>
   <si>
-    <t xml:space="preserve">Game 3 </t>
-  </si>
-  <si>
     <t>Game 4</t>
   </si>
   <si>
-    <t xml:space="preserve">Game 5 </t>
-  </si>
-  <si>
     <t>Game 6</t>
   </si>
   <si>
@@ -160,13 +148,25 @@
   </si>
   <si>
     <t xml:space="preserve">mentioned assuming that he wasn’t paired by the end of the experiment </t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Game 1</t>
+  </si>
+  <si>
+    <t>Game 3</t>
+  </si>
+  <si>
+    <t>Game 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -289,7 +289,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -324,7 +323,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -500,15 +498,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N44" sqref="N44"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
@@ -517,7 +515,7 @@
     <col min="14" max="14" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -537,31 +535,31 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L1" t="s">
         <v>9</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" t="s">
-        <v>13</v>
       </c>
       <c r="M1" t="s">
         <v>6</v>
       </c>
       <c r="N1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="1">
         <v>42055</v>
       </c>
@@ -569,7 +567,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <v>382</v>
@@ -599,13 +597,13 @@
         <v>98</v>
       </c>
       <c r="M2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="N2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="1">
         <v>42057</v>
       </c>
@@ -613,43 +611,43 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D3">
         <v>383</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F3">
         <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="K3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="L3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="M3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="N3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="1">
         <v>42058</v>
       </c>
@@ -657,7 +655,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <v>384</v>
@@ -687,10 +685,10 @@
         <v>63</v>
       </c>
       <c r="M4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="1">
         <v>42058</v>
       </c>
@@ -698,7 +696,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D5">
         <v>385</v>
@@ -728,10 +726,10 @@
         <v>0</v>
       </c>
       <c r="M5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="1">
         <v>42058</v>
       </c>
@@ -739,7 +737,7 @@
         <v>0.625</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <v>386</v>
@@ -769,10 +767,10 @@
         <v>73</v>
       </c>
       <c r="M6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="1">
         <v>42058</v>
       </c>
@@ -780,7 +778,7 @@
         <v>0.625</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D7">
         <v>387</v>
@@ -810,10 +808,10 @@
         <v>0</v>
       </c>
       <c r="M7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="1">
         <v>42060</v>
       </c>
@@ -821,7 +819,7 @@
         <v>0.625</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D8">
         <v>388</v>
@@ -851,10 +849,10 @@
         <v>125</v>
       </c>
       <c r="M8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="1">
         <v>42060</v>
       </c>
@@ -862,7 +860,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D9">
         <v>389</v>
@@ -892,10 +890,10 @@
         <v>0</v>
       </c>
       <c r="M9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="1">
         <v>42060</v>
       </c>
@@ -903,7 +901,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D10">
         <v>390</v>
@@ -933,10 +931,10 @@
         <v>83</v>
       </c>
       <c r="M10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="1">
         <v>42062</v>
       </c>
@@ -944,7 +942,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D11">
         <v>391</v>
@@ -974,13 +972,13 @@
         <v>0</v>
       </c>
       <c r="M11" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="N11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="1">
         <v>42062</v>
       </c>
@@ -988,7 +986,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D12">
         <v>392</v>
@@ -1018,13 +1016,13 @@
         <v>61</v>
       </c>
       <c r="M12" t="s">
+        <v>17</v>
+      </c>
+      <c r="N12" t="s">
         <v>21</v>
       </c>
-      <c r="N12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="1">
         <v>42062</v>
       </c>
@@ -1032,7 +1030,7 @@
         <v>0.625</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D13">
         <v>393</v>
@@ -1062,13 +1060,13 @@
         <v>0</v>
       </c>
       <c r="M13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="N13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="1">
         <v>42062</v>
       </c>
@@ -1076,7 +1074,7 @@
         <v>0.625</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D14">
         <v>394</v>
@@ -1106,13 +1104,13 @@
         <v>82</v>
       </c>
       <c r="M14" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="N14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" s="1">
         <v>42069</v>
       </c>
@@ -1120,7 +1118,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D15">
         <v>395</v>
@@ -1150,10 +1148,10 @@
         <v>0</v>
       </c>
       <c r="M15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" s="1">
         <v>42069</v>
       </c>
@@ -1161,7 +1159,7 @@
         <v>0.625</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D16">
         <v>396</v>
@@ -1191,10 +1189,10 @@
         <v>27</v>
       </c>
       <c r="M16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="1">
         <v>42069</v>
       </c>
@@ -1202,7 +1200,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D17">
         <v>397</v>
@@ -1232,10 +1230,10 @@
         <v>0</v>
       </c>
       <c r="M17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="1">
         <v>42069</v>
       </c>
@@ -1243,7 +1241,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D18">
         <v>398</v>
@@ -1273,10 +1271,10 @@
         <v>69</v>
       </c>
       <c r="M18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="1">
         <v>42072</v>
       </c>
@@ -1284,7 +1282,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C19" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D19">
         <v>399</v>
@@ -1314,10 +1312,10 @@
         <v>0</v>
       </c>
       <c r="M19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="1">
         <v>42072</v>
       </c>
@@ -1325,7 +1323,7 @@
         <v>0.625</v>
       </c>
       <c r="C20" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D20">
         <v>400</v>
@@ -1355,10 +1353,10 @@
         <v>30</v>
       </c>
       <c r="M20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="1">
         <v>42074</v>
       </c>
@@ -1366,7 +1364,7 @@
         <v>0.625</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D21">
         <v>401</v>
@@ -1396,10 +1394,10 @@
         <v>0</v>
       </c>
       <c r="M21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" s="1">
         <v>42074</v>
       </c>
@@ -1407,7 +1405,7 @@
         <v>0.625</v>
       </c>
       <c r="C22" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D22">
         <v>402</v>
@@ -1437,10 +1435,10 @@
         <v>104</v>
       </c>
       <c r="M22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" s="1">
         <v>42074</v>
       </c>
@@ -1448,7 +1446,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C23" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D23">
         <v>403</v>
@@ -1478,13 +1476,13 @@
         <v>0</v>
       </c>
       <c r="M23" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="N23" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" s="1">
         <v>42076</v>
       </c>
@@ -1492,7 +1490,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C24" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D24">
         <v>404</v>
@@ -1522,13 +1520,13 @@
         <v>87</v>
       </c>
       <c r="M24" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="N24" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" s="1">
         <v>42076</v>
       </c>
@@ -1536,7 +1534,7 @@
         <v>0.625</v>
       </c>
       <c r="C25" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D25">
         <v>405</v>
@@ -1566,13 +1564,13 @@
         <v>0</v>
       </c>
       <c r="M25" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="N25" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" s="1">
         <v>42079</v>
       </c>
@@ -1580,7 +1578,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D26">
         <v>406</v>
@@ -1610,10 +1608,10 @@
         <v>47</v>
       </c>
       <c r="M26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" s="1">
         <v>42079</v>
       </c>
@@ -1621,7 +1619,7 @@
         <v>0.625</v>
       </c>
       <c r="C27" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D27">
         <v>407</v>
@@ -1651,13 +1649,13 @@
         <v>0</v>
       </c>
       <c r="M27" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="N27" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" s="1">
         <v>42081</v>
       </c>
@@ -1665,7 +1663,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C28" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D28">
         <v>408</v>
@@ -1695,13 +1693,13 @@
         <v>43</v>
       </c>
       <c r="M28" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="N28" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" s="1">
         <v>42081</v>
       </c>
@@ -1709,7 +1707,7 @@
         <v>0.625</v>
       </c>
       <c r="C29" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D29">
         <v>409</v>
@@ -1739,13 +1737,13 @@
         <v>0</v>
       </c>
       <c r="M29" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="N29" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" s="1">
         <v>42081</v>
       </c>
@@ -1753,7 +1751,7 @@
         <v>0.625</v>
       </c>
       <c r="C30" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D30">
         <v>410</v>
@@ -1783,13 +1781,13 @@
         <v>50</v>
       </c>
       <c r="M30" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="N30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
       <c r="A31" s="1">
         <v>42081</v>
       </c>
@@ -1797,7 +1795,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C31" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D31">
         <v>411</v>
@@ -1827,13 +1825,13 @@
         <v>0</v>
       </c>
       <c r="M31" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="N31" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
       <c r="A32" s="1">
         <v>42083</v>
       </c>
@@ -1841,7 +1839,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C32" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D32">
         <v>412</v>
@@ -1871,13 +1869,13 @@
         <v>67</v>
       </c>
       <c r="M32" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="N32" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
       <c r="A33" s="1">
         <v>42095</v>
       </c>
@@ -1885,7 +1883,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C33" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D33">
         <v>413</v>
@@ -1915,10 +1913,10 @@
         <v>0</v>
       </c>
       <c r="M33" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
       <c r="A34" s="1">
         <v>42095</v>
       </c>
@@ -1926,7 +1924,7 @@
         <v>0.625</v>
       </c>
       <c r="C34" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D34">
         <v>414</v>
@@ -1956,10 +1954,10 @@
         <v>126</v>
       </c>
       <c r="M34" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
       <c r="A35" s="1">
         <v>42095</v>
       </c>
@@ -1967,7 +1965,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C35" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D35">
         <v>415</v>
@@ -1997,10 +1995,10 @@
         <v>0</v>
       </c>
       <c r="M35" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
       <c r="A36" s="1">
         <v>42095</v>
       </c>
@@ -2008,7 +2006,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C36" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D36">
         <v>416</v>
@@ -2038,10 +2036,10 @@
         <v>160</v>
       </c>
       <c r="M36" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
       <c r="A37" s="1">
         <v>42097</v>
       </c>
@@ -2049,7 +2047,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C37" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D37">
         <v>417</v>
@@ -2079,13 +2077,13 @@
         <v>0</v>
       </c>
       <c r="M37" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N37" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
       <c r="A38" s="1">
         <v>42097</v>
       </c>
@@ -2093,7 +2091,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C38" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D38">
         <v>418</v>
@@ -2123,13 +2121,13 @@
         <v>74</v>
       </c>
       <c r="M38" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="N38" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
       <c r="A39" s="1">
         <v>42097</v>
       </c>
@@ -2137,7 +2135,7 @@
         <v>0.625</v>
       </c>
       <c r="C39" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D39">
         <v>419</v>
@@ -2167,10 +2165,10 @@
         <v>0</v>
       </c>
       <c r="M39" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
       <c r="A40" s="1">
         <v>42097</v>
       </c>
@@ -2178,7 +2176,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C40" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D40">
         <v>420</v>
@@ -2208,13 +2206,13 @@
         <v>53</v>
       </c>
       <c r="M40" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="N40" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
       <c r="A41" s="1">
         <v>42102</v>
       </c>
@@ -2222,7 +2220,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C41" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D41">
         <v>421</v>
@@ -2252,10 +2250,10 @@
         <v>0</v>
       </c>
       <c r="M41" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
       <c r="A42" s="1">
         <v>42102</v>
       </c>
@@ -2263,7 +2261,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C42" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D42">
         <v>422</v>
@@ -2293,13 +2291,13 @@
         <v>116</v>
       </c>
       <c r="M42" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="N42" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
       <c r="A43" s="1">
         <v>42102</v>
       </c>
@@ -2307,7 +2305,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C43" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D43">
         <v>423</v>
@@ -2337,10 +2335,10 @@
         <v>0</v>
       </c>
       <c r="M43" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
       <c r="A44" s="1">
         <v>42102</v>
       </c>
@@ -2348,7 +2346,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C44" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D44">
         <v>424</v>
@@ -2378,7 +2376,7 @@
         <v>53</v>
       </c>
       <c r="M44" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -2388,24 +2386,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rachel did a lot of data entry, bless her.
</commit_message>
<xml_diff>
--- a/raw-data-prep/raw_data/Note_sheet_RP.xlsx
+++ b/raw-data-prep/raw_data/Note_sheet_RP.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
@@ -150,23 +150,23 @@
     <t xml:space="preserve">mentioned assuming that he wasn’t paired by the end of the experiment </t>
   </si>
   <si>
+    <t>Game 1</t>
+  </si>
+  <si>
+    <t>Game 3</t>
+  </si>
+  <si>
+    <t>Game 5</t>
+  </si>
+  <si>
     <t>Notes</t>
-  </si>
-  <si>
-    <t>Game 1</t>
-  </si>
-  <si>
-    <t>Game 3</t>
-  </si>
-  <si>
-    <t>Game 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -289,6 +289,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -323,6 +324,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -498,15 +500,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O1" sqref="O1"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
@@ -515,7 +517,7 @@
     <col min="14" max="14" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -535,19 +537,19 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J1" t="s">
         <v>8</v>
       </c>
       <c r="K1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L1" t="s">
         <v>9</v>
@@ -556,10 +558,10 @@
         <v>6</v>
       </c>
       <c r="N1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>42055</v>
       </c>
@@ -603,7 +605,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>42057</v>
       </c>
@@ -647,7 +649,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>42058</v>
       </c>
@@ -688,7 +690,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>42058</v>
       </c>
@@ -729,7 +731,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>42058</v>
       </c>
@@ -770,7 +772,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>42058</v>
       </c>
@@ -811,7 +813,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>42060</v>
       </c>
@@ -852,7 +854,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>42060</v>
       </c>
@@ -893,7 +895,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>42060</v>
       </c>
@@ -934,7 +936,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>42062</v>
       </c>
@@ -978,7 +980,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>42062</v>
       </c>
@@ -1022,7 +1024,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>42062</v>
       </c>
@@ -1066,7 +1068,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>42062</v>
       </c>
@@ -1110,7 +1112,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>42069</v>
       </c>
@@ -1151,7 +1153,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>42069</v>
       </c>
@@ -1192,7 +1194,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>42069</v>
       </c>
@@ -1233,7 +1235,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>42069</v>
       </c>
@@ -1274,7 +1276,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>42072</v>
       </c>
@@ -1315,7 +1317,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>42072</v>
       </c>
@@ -1356,7 +1358,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>42074</v>
       </c>
@@ -1397,7 +1399,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>42074</v>
       </c>
@@ -1438,7 +1440,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>42074</v>
       </c>
@@ -1482,7 +1484,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>42076</v>
       </c>
@@ -1526,7 +1528,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>42076</v>
       </c>
@@ -1570,7 +1572,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>42079</v>
       </c>
@@ -1611,7 +1613,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>42079</v>
       </c>
@@ -1655,7 +1657,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>42081</v>
       </c>
@@ -1699,7 +1701,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>42081</v>
       </c>
@@ -1743,7 +1745,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>42081</v>
       </c>
@@ -1787,7 +1789,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>42081</v>
       </c>
@@ -1831,7 +1833,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>42083</v>
       </c>
@@ -1875,7 +1877,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>42095</v>
       </c>
@@ -1916,7 +1918,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>42095</v>
       </c>
@@ -1957,7 +1959,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>42095</v>
       </c>
@@ -1998,7 +2000,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>42095</v>
       </c>
@@ -2039,7 +2041,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>42097</v>
       </c>
@@ -2083,7 +2085,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>42097</v>
       </c>
@@ -2127,7 +2129,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>42097</v>
       </c>
@@ -2168,7 +2170,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>42097</v>
       </c>
@@ -2212,7 +2214,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>42102</v>
       </c>
@@ -2253,7 +2255,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>42102</v>
       </c>
@@ -2297,7 +2299,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42102</v>
       </c>
@@ -2338,7 +2340,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42102</v>
       </c>
@@ -2386,24 +2388,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Further data entry by Rachel. Is this all of it?
</commit_message>
<xml_diff>
--- a/raw-data-prep/raw_data/Note_sheet_RP.xlsx
+++ b/raw-data-prep/raw_data/Note_sheet_RP.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="64">
   <si>
     <t>Subject</t>
   </si>
@@ -160,13 +160,61 @@
   </si>
   <si>
     <t>Good.Session</t>
+  </si>
+  <si>
+    <t>said near the end he was a little suspicious of the essay evaluations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subject was quiet </t>
+  </si>
+  <si>
+    <t xml:space="preserve">participant died on 1st level twice </t>
+  </si>
+  <si>
+    <t xml:space="preserve">said the evaluation seemed to harsh to be real </t>
+  </si>
+  <si>
+    <t xml:space="preserve">felt like ther may have been a fake partner after reading insults </t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">showed dissapointment when told we werent going to continue with the distraction task </t>
+  </si>
+  <si>
+    <t xml:space="preserve">said after the evaluation he knew that it was fake and if he had picked pro life he would've got a pro-choice essay back because they were probably fake </t>
+  </si>
+  <si>
+    <t xml:space="preserve">subject stated ge was suspicious tat the iinsult evaluation was a fake during funneled debriefing. He said it was because the evaluation was unrealistically harsh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">he didn’t explicitly say that he knew what was going on but he didn’t seem surprised at all and did say the evaluation seemed fishy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">said it was on of the most violent games hes played; said insults were super mean, so he got a little skeptical </t>
+  </si>
+  <si>
+    <t xml:space="preserve">said insults were a;; negatives so either the other guy was really mean or we were trying to pull something </t>
+  </si>
+  <si>
+    <t xml:space="preserve">said he had a few suspicions after skipping the distraction assignment even after testing the water </t>
+  </si>
+  <si>
+    <t xml:space="preserve">said that the evaluation seemed kind of weird. After being debriefed the subject said he was genuinely surprised about everything and "we had got him" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">said insults were really mean and kind of made him think it was fake </t>
+  </si>
+  <si>
+    <t xml:space="preserve">said he's done a study very similar to this, so he assumed he wasn’t paired with anyone </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -289,6 +337,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -323,6 +372,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -498,15 +548,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:N1"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
@@ -515,7 +565,7 @@
     <col min="14" max="14" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -559,7 +609,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>42055</v>
       </c>
@@ -603,7 +653,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>42057</v>
       </c>
@@ -647,7 +697,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>42058</v>
       </c>
@@ -688,7 +738,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>42058</v>
       </c>
@@ -729,7 +779,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>42058</v>
       </c>
@@ -770,7 +820,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>42058</v>
       </c>
@@ -811,7 +861,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>42060</v>
       </c>
@@ -852,7 +902,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>42060</v>
       </c>
@@ -893,7 +943,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>42060</v>
       </c>
@@ -934,7 +984,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>42062</v>
       </c>
@@ -978,7 +1028,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>42062</v>
       </c>
@@ -1022,7 +1072,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>42062</v>
       </c>
@@ -1066,7 +1116,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>42062</v>
       </c>
@@ -1110,7 +1160,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>42069</v>
       </c>
@@ -1151,7 +1201,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>42069</v>
       </c>
@@ -1192,7 +1242,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>42069</v>
       </c>
@@ -1233,7 +1283,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>42069</v>
       </c>
@@ -1274,7 +1324,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>42072</v>
       </c>
@@ -1315,7 +1365,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>42072</v>
       </c>
@@ -1356,7 +1406,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>42074</v>
       </c>
@@ -1397,7 +1447,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>42074</v>
       </c>
@@ -1438,7 +1488,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>42074</v>
       </c>
@@ -1482,7 +1532,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>42076</v>
       </c>
@@ -1526,7 +1576,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>42076</v>
       </c>
@@ -1570,7 +1620,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>42079</v>
       </c>
@@ -1611,7 +1661,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>42079</v>
       </c>
@@ -1655,7 +1705,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>42081</v>
       </c>
@@ -1699,7 +1749,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>42081</v>
       </c>
@@ -1743,7 +1793,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>42081</v>
       </c>
@@ -1787,7 +1837,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>42081</v>
       </c>
@@ -1831,7 +1881,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>42083</v>
       </c>
@@ -1875,7 +1925,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>42095</v>
       </c>
@@ -1916,7 +1966,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>42095</v>
       </c>
@@ -1957,7 +2007,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>42095</v>
       </c>
@@ -1998,7 +2048,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>42095</v>
       </c>
@@ -2039,7 +2089,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>42097</v>
       </c>
@@ -2083,7 +2133,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>42097</v>
       </c>
@@ -2127,7 +2177,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>42097</v>
       </c>
@@ -2168,7 +2218,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>42097</v>
       </c>
@@ -2212,7 +2262,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>42102</v>
       </c>
@@ -2253,7 +2303,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>42102</v>
       </c>
@@ -2297,7 +2347,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42102</v>
       </c>
@@ -2338,7 +2388,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42102</v>
       </c>
@@ -2377,6 +2427,953 @@
       </c>
       <c r="M44" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>42104</v>
+      </c>
+      <c r="B45" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45">
+        <v>425</v>
+      </c>
+      <c r="E45">
+        <v>4</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>446</v>
+      </c>
+      <c r="I45">
+        <v>22</v>
+      </c>
+      <c r="J45">
+        <v>2146</v>
+      </c>
+      <c r="K45">
+        <v>87</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+      <c r="M45" t="s">
+        <v>7</v>
+      </c>
+      <c r="N45" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>42104</v>
+      </c>
+      <c r="B46" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46">
+        <v>426</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46">
+        <v>2</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46">
+        <v>202</v>
+      </c>
+      <c r="I46">
+        <v>4</v>
+      </c>
+      <c r="J46">
+        <v>797</v>
+      </c>
+      <c r="K46">
+        <v>85</v>
+      </c>
+      <c r="L46">
+        <v>56</v>
+      </c>
+      <c r="M46" t="s">
+        <v>13</v>
+      </c>
+      <c r="N46" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>42104</v>
+      </c>
+      <c r="B47" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="C47" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47">
+        <v>427</v>
+      </c>
+      <c r="E47">
+        <v>4</v>
+      </c>
+      <c r="F47">
+        <v>3</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>603</v>
+      </c>
+      <c r="I47">
+        <v>20</v>
+      </c>
+      <c r="J47">
+        <v>49</v>
+      </c>
+      <c r="K47">
+        <v>515</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
+      <c r="M47" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>42104</v>
+      </c>
+      <c r="B48" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="C48" t="s">
+        <v>16</v>
+      </c>
+      <c r="D48">
+        <v>428</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48">
+        <v>4</v>
+      </c>
+      <c r="G48">
+        <v>14</v>
+      </c>
+      <c r="H48">
+        <v>232</v>
+      </c>
+      <c r="I48">
+        <v>3</v>
+      </c>
+      <c r="J48">
+        <v>214</v>
+      </c>
+      <c r="K48">
+        <v>138</v>
+      </c>
+      <c r="L48">
+        <v>181</v>
+      </c>
+      <c r="M48" t="s">
+        <v>13</v>
+      </c>
+      <c r="N48" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>42104</v>
+      </c>
+      <c r="B49" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C49" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49">
+        <v>429</v>
+      </c>
+      <c r="E49">
+        <v>4</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>206</v>
+      </c>
+      <c r="I49">
+        <v>7</v>
+      </c>
+      <c r="J49">
+        <v>37</v>
+      </c>
+      <c r="K49">
+        <v>219</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="M49" t="s">
+        <v>7</v>
+      </c>
+      <c r="N49" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>42109</v>
+      </c>
+      <c r="B50" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50">
+        <v>430</v>
+      </c>
+      <c r="E50">
+        <v>4</v>
+      </c>
+      <c r="F50">
+        <v>2</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>311</v>
+      </c>
+      <c r="I50">
+        <v>10</v>
+      </c>
+      <c r="J50">
+        <v>1118</v>
+      </c>
+      <c r="K50">
+        <v>70</v>
+      </c>
+      <c r="L50">
+        <v>47</v>
+      </c>
+      <c r="M50" t="s">
+        <v>7</v>
+      </c>
+      <c r="N50" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>42109</v>
+      </c>
+      <c r="B51" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="C51" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51">
+        <v>431</v>
+      </c>
+      <c r="E51">
+        <v>4</v>
+      </c>
+      <c r="F51">
+        <v>3</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>471</v>
+      </c>
+      <c r="I51">
+        <v>16</v>
+      </c>
+      <c r="J51">
+        <v>515</v>
+      </c>
+      <c r="K51">
+        <v>322</v>
+      </c>
+      <c r="L51">
+        <v>0</v>
+      </c>
+      <c r="M51" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>42109</v>
+      </c>
+      <c r="B52" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="C52" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52">
+        <v>432</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52">
+        <v>4</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>411</v>
+      </c>
+      <c r="I52">
+        <v>13</v>
+      </c>
+      <c r="J52">
+        <v>1450</v>
+      </c>
+      <c r="K52">
+        <v>127</v>
+      </c>
+      <c r="L52">
+        <v>84</v>
+      </c>
+      <c r="M52" t="s">
+        <v>53</v>
+      </c>
+      <c r="N52" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>42109</v>
+      </c>
+      <c r="B53" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C53" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53">
+        <v>433</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>436</v>
+      </c>
+      <c r="I53">
+        <v>14</v>
+      </c>
+      <c r="J53">
+        <v>2614</v>
+      </c>
+      <c r="K53">
+        <v>6</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+      <c r="M53" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>42109</v>
+      </c>
+      <c r="B54" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C54" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54">
+        <v>434</v>
+      </c>
+      <c r="E54">
+        <v>4</v>
+      </c>
+      <c r="F54">
+        <v>2</v>
+      </c>
+      <c r="G54">
+        <v>4</v>
+      </c>
+      <c r="H54">
+        <v>383</v>
+      </c>
+      <c r="I54">
+        <v>6</v>
+      </c>
+      <c r="J54">
+        <v>1464</v>
+      </c>
+      <c r="K54">
+        <v>92</v>
+      </c>
+      <c r="L54">
+        <v>126</v>
+      </c>
+      <c r="M54" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>42111</v>
+      </c>
+      <c r="B55" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="C55" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55">
+        <v>435</v>
+      </c>
+      <c r="E55">
+        <v>2</v>
+      </c>
+      <c r="F55">
+        <v>3</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>459</v>
+      </c>
+      <c r="I55">
+        <v>15</v>
+      </c>
+      <c r="J55">
+        <v>2240</v>
+      </c>
+      <c r="K55">
+        <v>56</v>
+      </c>
+      <c r="L55">
+        <v>0</v>
+      </c>
+      <c r="M55" t="s">
+        <v>18</v>
+      </c>
+      <c r="N55" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>42111</v>
+      </c>
+      <c r="B56" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="C56" t="s">
+        <v>16</v>
+      </c>
+      <c r="D56">
+        <v>436</v>
+      </c>
+      <c r="E56">
+        <v>4</v>
+      </c>
+      <c r="F56">
+        <v>4</v>
+      </c>
+      <c r="G56">
+        <v>6</v>
+      </c>
+      <c r="H56">
+        <v>288</v>
+      </c>
+      <c r="I56">
+        <v>3</v>
+      </c>
+      <c r="J56">
+        <v>1181</v>
+      </c>
+      <c r="K56">
+        <v>72</v>
+      </c>
+      <c r="L56">
+        <v>116</v>
+      </c>
+      <c r="M56" t="s">
+        <v>7</v>
+      </c>
+      <c r="N56" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>42111</v>
+      </c>
+      <c r="B57" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C57" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57">
+        <v>437</v>
+      </c>
+      <c r="E57">
+        <v>4</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>485</v>
+      </c>
+      <c r="I57">
+        <v>22</v>
+      </c>
+      <c r="J57">
+        <v>670</v>
+      </c>
+      <c r="K57">
+        <v>240</v>
+      </c>
+      <c r="L57">
+        <v>0</v>
+      </c>
+      <c r="M57" t="s">
+        <v>7</v>
+      </c>
+      <c r="N57" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>42116</v>
+      </c>
+      <c r="B58" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="C58" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58">
+        <v>438</v>
+      </c>
+      <c r="E58">
+        <v>4</v>
+      </c>
+      <c r="F58">
+        <v>2</v>
+      </c>
+      <c r="G58">
+        <v>2</v>
+      </c>
+      <c r="H58">
+        <v>263</v>
+      </c>
+      <c r="I58">
+        <v>3</v>
+      </c>
+      <c r="J58">
+        <v>1031</v>
+      </c>
+      <c r="K58">
+        <v>52</v>
+      </c>
+      <c r="L58">
+        <v>64</v>
+      </c>
+      <c r="M58" t="s">
+        <v>7</v>
+      </c>
+      <c r="N58" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>42116</v>
+      </c>
+      <c r="B59" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C59" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59">
+        <v>439</v>
+      </c>
+      <c r="E59">
+        <v>4</v>
+      </c>
+      <c r="F59">
+        <v>3</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>425</v>
+      </c>
+      <c r="I59">
+        <v>14</v>
+      </c>
+      <c r="J59">
+        <v>681</v>
+      </c>
+      <c r="K59">
+        <v>310</v>
+      </c>
+      <c r="L59">
+        <v>0</v>
+      </c>
+      <c r="M59" t="s">
+        <v>28</v>
+      </c>
+      <c r="N59" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>42116</v>
+      </c>
+      <c r="B60" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C60" t="s">
+        <v>9</v>
+      </c>
+      <c r="D60">
+        <v>440</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60">
+        <v>4</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>385</v>
+      </c>
+      <c r="I60">
+        <v>13</v>
+      </c>
+      <c r="J60">
+        <v>1958</v>
+      </c>
+      <c r="K60">
+        <v>77</v>
+      </c>
+      <c r="L60">
+        <v>78</v>
+      </c>
+      <c r="M60" t="s">
+        <v>7</v>
+      </c>
+      <c r="N60" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>42118</v>
+      </c>
+      <c r="B61" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="C61" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61">
+        <v>441</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61">
+        <v>1</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>444</v>
+      </c>
+      <c r="I61">
+        <v>22</v>
+      </c>
+      <c r="J61">
+        <v>612</v>
+      </c>
+      <c r="K61">
+        <v>264</v>
+      </c>
+      <c r="L61">
+        <v>0</v>
+      </c>
+      <c r="M61" t="s">
+        <v>13</v>
+      </c>
+      <c r="N61" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>42123</v>
+      </c>
+      <c r="B62" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="C62" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62">
+        <v>442</v>
+      </c>
+      <c r="E62">
+        <v>4</v>
+      </c>
+      <c r="F62">
+        <v>2</v>
+      </c>
+      <c r="G62">
+        <v>1</v>
+      </c>
+      <c r="H62">
+        <v>373</v>
+      </c>
+      <c r="I62">
+        <v>12</v>
+      </c>
+      <c r="J62">
+        <v>1419</v>
+      </c>
+      <c r="K62">
+        <v>124</v>
+      </c>
+      <c r="L62">
+        <v>56</v>
+      </c>
+      <c r="M62" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>42128</v>
+      </c>
+      <c r="B63" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="C63" t="s">
+        <v>22</v>
+      </c>
+      <c r="D63">
+        <v>443</v>
+      </c>
+      <c r="E63">
+        <v>4</v>
+      </c>
+      <c r="F63">
+        <v>3</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>392</v>
+      </c>
+      <c r="I63">
+        <v>17</v>
+      </c>
+      <c r="J63">
+        <v>991</v>
+      </c>
+      <c r="K63">
+        <v>183</v>
+      </c>
+      <c r="L63">
+        <v>0</v>
+      </c>
+      <c r="M63" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>42128</v>
+      </c>
+      <c r="B64" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C64" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64">
+        <v>444</v>
+      </c>
+      <c r="E64">
+        <v>4</v>
+      </c>
+      <c r="F64">
+        <v>4</v>
+      </c>
+      <c r="G64">
+        <v>1</v>
+      </c>
+      <c r="H64">
+        <v>440</v>
+      </c>
+      <c r="I64">
+        <v>12</v>
+      </c>
+      <c r="J64">
+        <v>1048</v>
+      </c>
+      <c r="K64">
+        <v>176</v>
+      </c>
+      <c r="L64">
+        <v>89</v>
+      </c>
+      <c r="M64" t="s">
+        <v>28</v>
+      </c>
+      <c r="N64" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>42130</v>
+      </c>
+      <c r="B65" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C65" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65">
+        <v>445</v>
+      </c>
+      <c r="E65">
+        <v>4</v>
+      </c>
+      <c r="F65">
+        <v>1</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>439</v>
+      </c>
+      <c r="I65">
+        <v>15</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+      <c r="K65">
+        <v>368</v>
+      </c>
+      <c r="L65">
+        <v>0</v>
+      </c>
+      <c r="M65" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>42130</v>
+      </c>
+      <c r="B66" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="C66" t="s">
+        <v>6</v>
+      </c>
+      <c r="D66">
+        <v>446</v>
+      </c>
+      <c r="E66">
+        <v>4</v>
+      </c>
+      <c r="F66">
+        <v>2</v>
+      </c>
+      <c r="G66">
+        <v>1</v>
+      </c>
+      <c r="H66">
+        <v>294</v>
+      </c>
+      <c r="I66">
+        <v>9</v>
+      </c>
+      <c r="J66">
+        <v>1176</v>
+      </c>
+      <c r="K66">
+        <v>72</v>
+      </c>
+      <c r="L66">
+        <v>59</v>
+      </c>
+      <c r="M66" t="s">
+        <v>18</v>
+      </c>
+      <c r="N66" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2386,24 +3383,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>